<commit_message>
Primera.3 versión de la aplicación
Commit 1.3 26-05-2025
</commit_message>
<xml_diff>
--- a/backend/electron_app/Biblioteca.xlsx
+++ b/backend/electron_app/Biblioteca.xlsx
@@ -4,8 +4,8 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="USUARIOS" sheetId="1" r:id="rId1"/>
-    <sheet name="PRESTAMOS" sheetId="2" r:id="rId2"/>
-    <sheet name="CATALOGO" sheetId="3" r:id="rId3"/>
+    <sheet name="CATALOGO" sheetId="2" r:id="rId2"/>
+    <sheet name="PRESTAMOS" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="str">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C4" t="str">
         <v>1</v>
@@ -476,16 +476,16 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -516,52 +516,44 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>1</v>
+      </c>
+      <c r="B9" t="str">
+        <v>1</v>
+      </c>
+      <c r="C9" t="str">
+        <v>1</v>
+      </c>
+      <c r="D9" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>1</v>
+      </c>
+      <c r="B10" t="str">
+        <v>1</v>
+      </c>
+      <c r="C10" t="str">
+        <v>1</v>
+      </c>
+      <c r="D10" t="str">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>ID_PRESTAMO</v>
-      </c>
-      <c r="B1" t="str">
-        <v>ID_EJEMPLAR_FK</v>
-      </c>
-      <c r="C1" t="str">
-        <v>RUT_FK</v>
-      </c>
-      <c r="D1" t="str">
-        <v>FECHA_PRESTAMO</v>
-      </c>
-      <c r="E1" t="str">
-        <v>FECHA_DEVOLUCION</v>
-      </c>
-      <c r="F1" t="str">
-        <v>ESTADO_ENTREGA</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -600,298 +592,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>123</v>
-      </c>
-      <c r="B3" t="str">
-        <v>123</v>
-      </c>
-      <c r="C3" t="str">
-        <v>123</v>
-      </c>
-      <c r="D3" t="str">
-        <v>123</v>
-      </c>
-      <c r="E3" t="str">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>123</v>
-      </c>
-      <c r="B4" t="str">
-        <v>123</v>
-      </c>
-      <c r="C4" t="str">
-        <v>123</v>
-      </c>
-      <c r="D4" t="str">
-        <v>123</v>
-      </c>
-      <c r="E4" t="str">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>123</v>
-      </c>
-      <c r="B5" t="str">
-        <v>123</v>
-      </c>
-      <c r="C5" t="str">
-        <v>123</v>
-      </c>
-      <c r="D5" t="str">
-        <v>123</v>
-      </c>
-      <c r="E5" t="str">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>123</v>
-      </c>
-      <c r="B6" t="str">
-        <v>123</v>
-      </c>
-      <c r="C6" t="str">
-        <v>123</v>
-      </c>
-      <c r="D6" t="str">
-        <v>123</v>
-      </c>
-      <c r="E6" t="str">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="B7" t="str">
-        <v>003598X</v>
-      </c>
-      <c r="C7" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="D7" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="E7" t="str">
-        <v>9789500419574</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="B8" t="str">
-        <v>003598X</v>
-      </c>
-      <c r="C8" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="D8" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="E8" t="str">
-        <v>9789500419574</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="B9" t="str">
-        <v>003598X</v>
-      </c>
-      <c r="C9" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="D9" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="E9" t="str">
-        <v>9789500419574</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="B10" t="str">
-        <v>003598X</v>
-      </c>
-      <c r="C10" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="D10" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="E10" t="str">
-        <v>9789500419574</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="B11" t="str">
-        <v>003598X</v>
-      </c>
-      <c r="C11" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="D11" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="E11" t="str">
-        <v>9789500419574</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="B12" t="str">
-        <v>003598X</v>
-      </c>
-      <c r="C12" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="D12" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="E12" t="str">
-        <v>9789500419574</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="B13" t="str">
-        <v>003598X</v>
-      </c>
-      <c r="C13" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="D13" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="E13" t="str">
-        <v>9789500419574</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="B14" t="str">
-        <v>003598X</v>
-      </c>
-      <c r="C14" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="D14" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="E14" t="str">
-        <v>9789500419574</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="B15" t="str">
-        <v>003598X</v>
-      </c>
-      <c r="C15" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="D15" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="E15" t="str">
-        <v>9789500419574</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="B16" t="str">
-        <v>003598X</v>
-      </c>
-      <c r="C16" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="D16" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="E16" t="str">
-        <v>9789500419574</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="B17" t="str">
-        <v>003598X</v>
-      </c>
-      <c r="C17" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="D17" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="E17" t="str">
-        <v>9789500419574</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="B18" t="str">
-        <v>003598X</v>
-      </c>
-      <c r="C18" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="D18" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="E18" t="str">
-        <v>9789500419574</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="B19" t="str">
-        <v>003598X</v>
-      </c>
-      <c r="C19" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="D19" t="str">
-        <v>9789500419574</v>
-      </c>
-      <c r="E19" t="str">
-        <v>9789500419574</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rendererPrestamos issue picking titulo
issue fixed by deleting
  searchInput.value = "";
in line 143-144
</commit_message>
<xml_diff>
--- a/backend/electron_app/Biblioteca.xlsx
+++ b/backend/electron_app/Biblioteca.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -420,140 +420,28 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>1</v>
-      </c>
-      <c r="B3" t="str">
-        <v>1</v>
-      </c>
-      <c r="C3" t="str">
-        <v>1</v>
-      </c>
-      <c r="D3" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>1</v>
-      </c>
-      <c r="B4" t="str">
-        <v>1</v>
-      </c>
-      <c r="C4" t="str">
-        <v>1</v>
-      </c>
-      <c r="D4" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>1</v>
-      </c>
-      <c r="B5" t="str">
-        <v>1</v>
-      </c>
-      <c r="C5" t="str">
-        <v>1</v>
-      </c>
-      <c r="D5" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>1</v>
-      </c>
-      <c r="B6" t="str">
-        <v>1</v>
-      </c>
-      <c r="C6" t="str">
-        <v>1</v>
-      </c>
-      <c r="D6" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>1</v>
-      </c>
-      <c r="B7" t="str">
-        <v>1</v>
-      </c>
-      <c r="C7" t="str">
-        <v>1</v>
-      </c>
-      <c r="D7" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>1</v>
-      </c>
-      <c r="B8" t="str">
-        <v>1</v>
-      </c>
-      <c r="C8" t="str">
-        <v>1</v>
-      </c>
-      <c r="D8" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>1</v>
-      </c>
-      <c r="B9" t="str">
-        <v>1</v>
-      </c>
-      <c r="C9" t="str">
-        <v>1</v>
-      </c>
-      <c r="D9" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>1</v>
-      </c>
-      <c r="B10" t="str">
-        <v>1</v>
-      </c>
-      <c r="C10" t="str">
-        <v>1</v>
-      </c>
-      <c r="D10" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -592,9 +480,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>1</v>
+      </c>
+      <c r="B3" t="str">
+        <v>1</v>
+      </c>
+      <c r="C3" t="str">
+        <v>1</v>
+      </c>
+      <c r="D3" t="str">
+        <v>1</v>
+      </c>
+      <c r="E3" t="str">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
busqueda en eliminar y editar con sus funciones hechas
</commit_message>
<xml_diff>
--- a/backend/electron_app/Biblioteca.xlsx
+++ b/backend/electron_app/Biblioteca.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -420,21 +420,119 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>1</v>
+      </c>
+      <c r="C2" t="str">
+        <v>1</v>
+      </c>
+      <c r="D2" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>1</v>
+      </c>
+      <c r="B3" t="str">
+        <v>1</v>
+      </c>
+      <c r="C3" t="str">
+        <v>1</v>
+      </c>
+      <c r="D3" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>1</v>
+      </c>
+      <c r="B4" t="str">
+        <v>1</v>
+      </c>
+      <c r="C4" t="str">
+        <v>1</v>
+      </c>
+      <c r="D4" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>1</v>
+      </c>
+      <c r="B5" t="str">
+        <v>1</v>
+      </c>
+      <c r="C5" t="str">
+        <v>1</v>
+      </c>
+      <c r="D5" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>1</v>
+      </c>
+      <c r="B6" t="str">
+        <v>1</v>
+      </c>
+      <c r="C6" t="str">
+        <v>1</v>
+      </c>
+      <c r="D6" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>1</v>
+      </c>
+      <c r="B7" t="str">
+        <v>1</v>
+      </c>
+      <c r="C7" t="str">
+        <v>1</v>
+      </c>
+      <c r="D7" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>1</v>
+      </c>
+      <c r="B8" t="str">
+        <v>1</v>
+      </c>
+      <c r="C8" t="str">
+        <v>1</v>
+      </c>
+      <c r="D8" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
         <v>2</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B9" t="str">
+        <v>3</v>
+      </c>
+      <c r="C9" t="str">
         <v>2</v>
       </c>
-      <c r="C2" t="str">
-        <v>2</v>
-      </c>
-      <c r="D2" t="str">
+      <c r="D9" t="str">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D9"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
error de freeze solucionado
</commit_message>
<xml_diff>
--- a/backend/electron_app/Biblioteca.xlsx
+++ b/backend/electron_app/Biblioteca.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -420,16 +420,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="str">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -446,93 +446,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>1</v>
-      </c>
-      <c r="B4" t="str">
-        <v>1</v>
-      </c>
-      <c r="C4" t="str">
-        <v>1</v>
-      </c>
-      <c r="D4" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>1</v>
-      </c>
-      <c r="B5" t="str">
-        <v>1</v>
-      </c>
-      <c r="C5" t="str">
-        <v>1</v>
-      </c>
-      <c r="D5" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>1</v>
-      </c>
-      <c r="B6" t="str">
-        <v>1</v>
-      </c>
-      <c r="C6" t="str">
-        <v>1</v>
-      </c>
-      <c r="D6" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>1</v>
-      </c>
-      <c r="B7" t="str">
-        <v>1</v>
-      </c>
-      <c r="C7" t="str">
-        <v>1</v>
-      </c>
-      <c r="D7" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>1</v>
-      </c>
-      <c r="B8" t="str">
-        <v>1</v>
-      </c>
-      <c r="C8" t="str">
-        <v>1</v>
-      </c>
-      <c r="D8" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>2</v>
-      </c>
-      <c r="B9" t="str">
-        <v>3</v>
-      </c>
-      <c r="C9" t="str">
-        <v>2</v>
-      </c>
-      <c r="D9" t="str">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>